<commit_message>
Fixing the verification steps for each sprint
</commit_message>
<xml_diff>
--- a/TestData_Registration.xlsx
+++ b/TestData_Registration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham Farrendy\git\CCN-Projects-Booking-Concierge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Cargo Community Network Pte Ltd\Booking Concierge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E04A71F-D5B0-4BCD-9F2B-D4685D6979B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64003991-5DEE-4410-BD37-B22AD1A9F0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13284" yWindow="36" windowWidth="9756" windowHeight="12552" xr2:uid="{4753EE7C-EBB4-4EF4-9500-BE846AFCB7DA}"/>
+    <workbookView xWindow="-120" yWindow="-15720" windowWidth="29040" windowHeight="15840" xr2:uid="{4753EE7C-EBB4-4EF4-9500-BE846AFCB7DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>password</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>TestAcc5</t>
+  </si>
+  <si>
+    <t>testfsd34</t>
+  </si>
+  <si>
+    <t>testingdevbcregression1@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -440,18 +446,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49BC636-F9FF-44ED-8F15-F52BB66C3487}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -471,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -491,8 +502,10 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -503,7 +516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -521,13 +534,19 @@
       </c>
       <c r="F4">
         <v>123556762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E2EB90BA-450F-4EB2-8143-0DE7E03F89D6}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{E4D2F683-6166-4F31-8567-39F9C672ED8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>